<commit_message>
Remove misformatted result folder
</commit_message>
<xml_diff>
--- a/Data/CDC_WONDER_4_YEAR_TOTAL.xlsx
+++ b/Data/CDC_WONDER_4_YEAR_TOTAL.xlsx
@@ -840,8 +840,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4F328AB88706D448AC78BA5EACD5868" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ea121367de00eb5315d214fb75588841">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d40583b3-3b49-46ec-a696-de629a5756ed" xmlns:ns3="38d181cc-8454-466e-9217-0c4239f5d1cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d41fcee84e32ab97fb0635623a484afb" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4F328AB88706D448AC78BA5EACD5868" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e9d9f6628cfd57a25ae655f4e89536d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d40583b3-3b49-46ec-a696-de629a5756ed" xmlns:ns3="38d181cc-8454-466e-9217-0c4239f5d1cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dc89e96ba85faf481da03e6bd35c85ea" ns2:_="" ns3:_="">
     <xsd:import namespace="d40583b3-3b49-46ec-a696-de629a5756ed"/>
     <xsd:import namespace="38d181cc-8454-466e-9217-0c4239f5d1cc"/>
     <xsd:element name="properties">
@@ -1097,7 +1097,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD42C2EC-3A41-4048-BFED-B86638FB4A12}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{105D9967-73B8-4052-B0DC-AB04725D606A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>